<commit_message>
add help update multi result
</commit_message>
<xml_diff>
--- a/bin/onmyoji.xlsx
+++ b/bin/onmyoji.xlsx
@@ -373,14 +373,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>이미지</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>인벤</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>특수</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -757,6 +749,14 @@
   </si>
   <si>
     <t>4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>정보페이지 URL</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>이미지 URL</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1476,7 +1476,7 @@
   <dimension ref="A1:H208"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12:F15"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1511,10 +1511,10 @@
         <v>94</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>96</v>
+        <v>193</v>
       </c>
       <c r="H1" s="6" t="s">
-        <v>95</v>
+        <v>194</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
@@ -1797,16 +1797,16 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" s="7" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="E20" s="3">
         <v>8</v>
@@ -1816,10 +1816,10 @@
       <c r="A21" s="7"/>
       <c r="B21" s="8"/>
       <c r="C21" s="3" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="E21" s="3">
         <v>8</v>
@@ -1829,10 +1829,10 @@
       <c r="A22" s="7"/>
       <c r="B22" s="8"/>
       <c r="C22" s="3" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="E22" s="3">
         <v>6</v>
@@ -1845,7 +1845,7 @@
         <v>53</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="E23" s="3">
         <v>6</v>
@@ -1858,7 +1858,7 @@
         <v>54</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="E24" s="3">
         <v>3</v>
@@ -1871,7 +1871,7 @@
         <v>54</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="E25" s="3">
         <v>6</v>
@@ -1884,7 +1884,7 @@
         <v>54</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="E26" s="3">
         <v>2</v>
@@ -1892,16 +1892,16 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" s="7" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B27" s="8" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="E27" s="3">
         <v>3</v>
@@ -1911,10 +1911,10 @@
       <c r="A28" s="7"/>
       <c r="B28" s="8"/>
       <c r="C28" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="D28" s="4" t="s">
         <v>150</v>
-      </c>
-      <c r="D28" s="4" t="s">
-        <v>152</v>
       </c>
       <c r="E28" s="3">
         <v>4</v>
@@ -1924,10 +1924,10 @@
       <c r="A29" s="7"/>
       <c r="B29" s="8"/>
       <c r="C29" s="3" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="E29" s="3">
         <v>4</v>
@@ -1935,16 +1935,16 @@
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" s="7" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B30" s="8" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="E30" s="3">
         <v>3</v>
@@ -1954,10 +1954,10 @@
       <c r="A31" s="7"/>
       <c r="B31" s="8"/>
       <c r="C31" s="3" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="E31" s="3">
         <v>1</v>
@@ -1967,10 +1967,10 @@
       <c r="A32" s="7"/>
       <c r="B32" s="8"/>
       <c r="C32" s="3" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="D32" s="4" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="E32" s="3">
         <v>2</v>
@@ -1980,10 +1980,10 @@
       <c r="A33" s="7"/>
       <c r="B33" s="8"/>
       <c r="C33" s="3" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="D33" s="4" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="E33" s="3">
         <v>2</v>
@@ -1991,16 +1991,16 @@
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" s="7" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B34" s="8" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="C34" s="3" t="s">
         <v>53</v>
       </c>
       <c r="D34" s="4" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="E34" s="3">
         <v>4</v>
@@ -2010,10 +2010,10 @@
       <c r="A35" s="7"/>
       <c r="B35" s="8"/>
       <c r="C35" s="3" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="D35" s="4" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="E35" s="3">
         <v>4</v>
@@ -2023,10 +2023,10 @@
       <c r="A36" s="7"/>
       <c r="B36" s="8"/>
       <c r="C36" s="3" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="D36" s="4" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="E36" s="3">
         <v>3</v>
@@ -2036,10 +2036,10 @@
       <c r="A37" s="7"/>
       <c r="B37" s="8"/>
       <c r="C37" s="3" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="D37" s="4" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="E37" s="3">
         <v>3</v>
@@ -2049,10 +2049,10 @@
       <c r="A38" s="7"/>
       <c r="B38" s="8"/>
       <c r="C38" s="3" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="D38" s="4" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="E38" s="3">
         <v>3</v>
@@ -2062,10 +2062,10 @@
       <c r="A39" s="7"/>
       <c r="B39" s="8"/>
       <c r="C39" s="3" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="D39" s="4" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="E39" s="3">
         <v>3</v>
@@ -2073,16 +2073,16 @@
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" s="7" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B40" s="8" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="D40" s="4" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="E40" s="3">
         <v>4</v>
@@ -2092,10 +2092,10 @@
       <c r="A41" s="7"/>
       <c r="B41" s="8"/>
       <c r="C41" s="3" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="D41" s="4" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="E41" s="3">
         <v>4</v>
@@ -2105,7 +2105,7 @@
       <c r="A42" s="7"/>
       <c r="B42" s="8"/>
       <c r="C42" s="3" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="D42" s="4" t="s">
         <v>31</v>
@@ -2118,10 +2118,10 @@
       <c r="A43" s="7"/>
       <c r="B43" s="8"/>
       <c r="C43" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="D43" s="4" t="s">
         <v>150</v>
-      </c>
-      <c r="D43" s="4" t="s">
-        <v>152</v>
       </c>
       <c r="E43" s="3">
         <v>4</v>
@@ -2131,10 +2131,10 @@
       <c r="A44" s="7"/>
       <c r="B44" s="8"/>
       <c r="C44" s="3" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="D44" s="4" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="E44" s="3">
         <v>2</v>
@@ -2142,16 +2142,16 @@
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45" s="7" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B45" s="8" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="D45" s="4" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="E45" s="3">
         <v>3</v>
@@ -2161,10 +2161,10 @@
       <c r="A46" s="7"/>
       <c r="B46" s="8"/>
       <c r="C46" s="3" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="D46" s="4" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="E46" s="3">
         <v>3</v>
@@ -2174,10 +2174,10 @@
       <c r="A47" s="7"/>
       <c r="B47" s="8"/>
       <c r="C47" s="3" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="D47" s="4" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="E47" s="3">
         <v>2</v>
@@ -2187,10 +2187,10 @@
       <c r="A48" s="7"/>
       <c r="B48" s="8"/>
       <c r="C48" s="3" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="D48" s="4" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="E48" s="3">
         <v>3</v>
@@ -2198,16 +2198,16 @@
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A49" s="7" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B49" s="8" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="C49" s="3" t="s">
         <v>54</v>
       </c>
       <c r="D49" s="4" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="E49" s="3">
         <v>4</v>
@@ -2217,10 +2217,10 @@
       <c r="A50" s="7"/>
       <c r="B50" s="8"/>
       <c r="C50" s="3" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="D50" s="4" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="E50" s="3">
         <v>1</v>
@@ -2230,10 +2230,10 @@
       <c r="A51" s="7"/>
       <c r="B51" s="8"/>
       <c r="C51" s="3" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="D51" s="4" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="E51" s="3">
         <v>4</v>
@@ -2241,16 +2241,16 @@
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A52" s="7" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B52" s="8" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="D52" s="4" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="E52" s="3">
         <v>7</v>
@@ -2263,7 +2263,7 @@
         <v>54</v>
       </c>
       <c r="D53" s="4" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="E53" s="3">
         <v>1</v>
@@ -2276,7 +2276,7 @@
         <v>54</v>
       </c>
       <c r="D54" s="4" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="E54" s="3">
         <v>1</v>
@@ -3297,13 +3297,13 @@
         <v>6</v>
       </c>
       <c r="B114" s="8" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C114" s="3" t="s">
         <v>53</v>
       </c>
       <c r="D114" s="4" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="E114" s="3">
         <v>3</v>
@@ -3313,10 +3313,10 @@
       <c r="A115" s="12"/>
       <c r="B115" s="8"/>
       <c r="C115" s="3" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="D115" s="4" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="E115" s="3">
         <v>4</v>
@@ -3326,10 +3326,10 @@
       <c r="A116" s="12"/>
       <c r="B116" s="8"/>
       <c r="C116" s="3" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="D116" s="4" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="E116" s="3">
         <v>3</v>
@@ -3339,10 +3339,10 @@
       <c r="A117" s="12"/>
       <c r="B117" s="8"/>
       <c r="C117" s="3" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="D117" s="4" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="E117" s="3">
         <v>1</v>
@@ -3352,10 +3352,10 @@
       <c r="A118" s="12"/>
       <c r="B118" s="8"/>
       <c r="C118" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="D118" s="4" t="s">
         <v>146</v>
-      </c>
-      <c r="D118" s="4" t="s">
-        <v>148</v>
       </c>
       <c r="E118" s="3">
         <v>1</v>
@@ -3366,13 +3366,13 @@
         <v>6</v>
       </c>
       <c r="B119" s="8" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C119" s="3" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="D119" s="4" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="E119" s="3">
         <v>8</v>
@@ -3382,10 +3382,10 @@
       <c r="A120" s="12"/>
       <c r="B120" s="8"/>
       <c r="C120" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="D120" s="4" t="s">
         <v>150</v>
-      </c>
-      <c r="D120" s="4" t="s">
-        <v>152</v>
       </c>
       <c r="E120" s="3">
         <v>3</v>
@@ -3395,10 +3395,10 @@
       <c r="A121" s="12"/>
       <c r="B121" s="8"/>
       <c r="C121" s="3" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="D121" s="4" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="E121" s="3">
         <v>5</v>
@@ -3409,13 +3409,13 @@
         <v>6</v>
       </c>
       <c r="B122" s="8" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C122" s="3" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="D122" s="4" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="E122" s="3">
         <v>5</v>
@@ -3425,10 +3425,10 @@
       <c r="A123" s="12"/>
       <c r="B123" s="8"/>
       <c r="C123" s="3" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="D123" s="4" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="E123" s="3">
         <v>1</v>
@@ -3439,13 +3439,13 @@
         <v>6</v>
       </c>
       <c r="B124" s="8" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C124" s="3" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="D124" s="4" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="E124" s="3">
         <v>1</v>
@@ -3455,10 +3455,10 @@
       <c r="A125" s="12"/>
       <c r="B125" s="8"/>
       <c r="C125" s="3" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="D125" s="4" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="E125" s="3">
         <v>1</v>
@@ -3468,10 +3468,10 @@
       <c r="A126" s="12"/>
       <c r="B126" s="8"/>
       <c r="C126" s="3" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="D126" s="4" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="E126" s="3">
         <v>2</v>
@@ -3482,13 +3482,13 @@
         <v>6</v>
       </c>
       <c r="B127" s="8" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C127" s="3" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="D127" s="4" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="E127" s="3">
         <v>1</v>
@@ -3498,10 +3498,10 @@
       <c r="A128" s="12"/>
       <c r="B128" s="8"/>
       <c r="C128" s="3" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="D128" s="4" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="E128" s="3">
         <v>6</v>
@@ -3511,10 +3511,10 @@
       <c r="A129" s="12"/>
       <c r="B129" s="8"/>
       <c r="C129" s="3" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="D129" s="4" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="E129" s="3">
         <v>2</v>
@@ -3525,13 +3525,13 @@
         <v>6</v>
       </c>
       <c r="B130" s="8" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C130" s="3" t="s">
         <v>54</v>
       </c>
       <c r="D130" s="4" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="E130" s="3">
         <v>1</v>
@@ -3544,7 +3544,7 @@
         <v>54</v>
       </c>
       <c r="D131" s="4" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="E131" s="3">
         <v>1</v>
@@ -3555,13 +3555,13 @@
         <v>6</v>
       </c>
       <c r="B132" s="8" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C132" s="3" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="D132" s="4" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="E132" s="3">
         <v>18</v>
@@ -3571,10 +3571,10 @@
       <c r="A133" s="12"/>
       <c r="B133" s="8"/>
       <c r="C133" s="3" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="D133" s="4" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="E133" s="3">
         <v>5</v>
@@ -3585,13 +3585,13 @@
         <v>6</v>
       </c>
       <c r="B134" s="8" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C134" s="3" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="D134" s="4" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="E134" s="3">
         <v>3</v>
@@ -3601,10 +3601,10 @@
       <c r="A135" s="12"/>
       <c r="B135" s="8"/>
       <c r="C135" s="3" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="D135" s="4" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="E135" s="3">
         <v>4</v>
@@ -3614,10 +3614,10 @@
       <c r="A136" s="12"/>
       <c r="B136" s="8"/>
       <c r="C136" s="3" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="D136" s="4" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="E136" s="3">
         <v>1</v>
@@ -3628,13 +3628,13 @@
         <v>6</v>
       </c>
       <c r="B137" s="8" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C137" s="3" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="D137" s="4" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="E137" s="3">
         <v>7</v>
@@ -3644,10 +3644,10 @@
       <c r="A138" s="12"/>
       <c r="B138" s="8"/>
       <c r="C138" s="3" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="D138" s="4" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="E138" s="3">
         <v>1</v>
@@ -3657,10 +3657,10 @@
       <c r="A139" s="12"/>
       <c r="B139" s="8"/>
       <c r="C139" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="D139" s="4" t="s">
         <v>162</v>
-      </c>
-      <c r="D139" s="4" t="s">
-        <v>164</v>
       </c>
       <c r="E139" s="3">
         <v>3</v>
@@ -3671,13 +3671,13 @@
         <v>6</v>
       </c>
       <c r="B140" s="2" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C140" s="3" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="D140" s="4" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="E140" s="3">
         <v>3</v>
@@ -3688,13 +3688,13 @@
         <v>6</v>
       </c>
       <c r="B141" s="8" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C141" s="3" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="D141" s="4" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="E141" s="3">
         <v>2</v>
@@ -3704,10 +3704,10 @@
       <c r="A142" s="12"/>
       <c r="B142" s="8"/>
       <c r="C142" s="3" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="D142" s="4" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="E142" s="3">
         <v>2</v>
@@ -3717,10 +3717,10 @@
       <c r="A143" s="12"/>
       <c r="B143" s="8"/>
       <c r="C143" s="3" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="D143" s="4" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="E143" s="3">
         <v>1</v>
@@ -4345,13 +4345,13 @@
         <v>24</v>
       </c>
       <c r="B180" s="8" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C180" s="3" t="s">
         <v>54</v>
       </c>
       <c r="D180" s="4" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="E180" s="3">
         <v>3</v>
@@ -4364,7 +4364,7 @@
         <v>54</v>
       </c>
       <c r="D181" s="4" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="E181" s="3">
         <v>1</v>
@@ -4375,13 +4375,13 @@
         <v>24</v>
       </c>
       <c r="B182" s="2" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C182" s="3" t="s">
         <v>54</v>
       </c>
       <c r="D182" s="4" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="E182" s="3">
         <v>2</v>
@@ -4392,13 +4392,13 @@
         <v>24</v>
       </c>
       <c r="B183" s="8" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C183" s="3" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="D183" s="4" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="E183" s="3">
         <v>1</v>
@@ -4411,7 +4411,7 @@
         <v>54</v>
       </c>
       <c r="D184" s="4" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="E184" s="3">
         <v>1</v>
@@ -4422,13 +4422,13 @@
         <v>24</v>
       </c>
       <c r="B185" s="8" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C185" s="3" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="D185" s="4" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="E185" s="3">
         <v>1</v>
@@ -4441,7 +4441,7 @@
         <v>54</v>
       </c>
       <c r="D186" s="4" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="E186" s="3">
         <v>1</v>
@@ -4454,7 +4454,7 @@
         <v>54</v>
       </c>
       <c r="D187" s="4" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="E187" s="3">
         <v>1</v>
@@ -4465,13 +4465,13 @@
         <v>24</v>
       </c>
       <c r="B188" s="2" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C188" s="3" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="D188" s="4" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="E188" s="3">
         <v>1</v>
@@ -4482,13 +4482,13 @@
         <v>24</v>
       </c>
       <c r="B189" s="8" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C189" s="3" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="D189" s="4" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="E189" s="3">
         <v>3</v>
@@ -4501,7 +4501,7 @@
         <v>54</v>
       </c>
       <c r="D190" s="4" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="E190" s="3">
         <v>10</v>
@@ -4514,7 +4514,7 @@
         <v>54</v>
       </c>
       <c r="D191" s="4" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="E191" s="3">
         <v>6</v>
@@ -4525,13 +4525,13 @@
         <v>24</v>
       </c>
       <c r="B192" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="C192" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="D192" s="4" t="s">
         <v>120</v>
-      </c>
-      <c r="C192" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="D192" s="4" t="s">
-        <v>122</v>
       </c>
       <c r="E192" s="3">
         <v>1</v>
@@ -4624,13 +4624,13 @@
         <v>38</v>
       </c>
       <c r="B198" s="2" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C198" s="3" t="s">
         <v>52</v>
       </c>
       <c r="D198" s="4" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="E198" s="3">
         <v>2</v>
@@ -4641,13 +4641,13 @@
         <v>38</v>
       </c>
       <c r="B199" s="8" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C199" s="3" t="s">
         <v>52</v>
       </c>
       <c r="D199" s="4" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="E199" s="3">
         <v>1</v>
@@ -4660,7 +4660,7 @@
         <v>52</v>
       </c>
       <c r="D200" s="4" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="E200" s="3">
         <v>1</v>
@@ -4673,7 +4673,7 @@
         <v>54</v>
       </c>
       <c r="D201" s="4" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="E201" s="3">
         <v>2</v>
@@ -4686,7 +4686,7 @@
         <v>54</v>
       </c>
       <c r="D202" s="4" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="E202" s="3">
         <v>1</v>
@@ -4697,13 +4697,13 @@
         <v>38</v>
       </c>
       <c r="B203" s="8" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C203" s="3" t="s">
         <v>52</v>
       </c>
       <c r="D203" s="4" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="E203" s="3">
         <v>2</v>
@@ -4716,7 +4716,7 @@
         <v>54</v>
       </c>
       <c r="D204" s="4" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="E204" s="3">
         <v>1</v>
@@ -4727,13 +4727,13 @@
         <v>38</v>
       </c>
       <c r="B205" s="2" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C205" s="3" t="s">
         <v>52</v>
       </c>
       <c r="D205" s="4" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="E205" s="3">
         <v>2</v>
@@ -4741,16 +4741,16 @@
     </row>
     <row r="206" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A206" s="2" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B206" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="C206" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="D206" s="4" t="s">
         <v>98</v>
-      </c>
-      <c r="C206" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="D206" s="4" t="s">
-        <v>100</v>
       </c>
       <c r="E206" s="3">
         <v>1</v>
@@ -4758,16 +4758,16 @@
     </row>
     <row r="207" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A207" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="B207" s="8" t="s">
         <v>97</v>
       </c>
-      <c r="B207" s="8" t="s">
+      <c r="C207" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="D207" s="4" t="s">
         <v>99</v>
-      </c>
-      <c r="C207" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="D207" s="4" t="s">
-        <v>101</v>
       </c>
       <c r="E207" s="3">
         <v>9</v>
@@ -4780,7 +4780,7 @@
         <v>54</v>
       </c>
       <c r="D208" s="4" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="E208" s="3">
         <v>2</v>
@@ -4788,56 +4788,49 @@
     </row>
   </sheetData>
   <mergeCells count="128">
-    <mergeCell ref="F55:F57"/>
-    <mergeCell ref="F58:F63"/>
-    <mergeCell ref="F68:F69"/>
-    <mergeCell ref="A193:A196"/>
-    <mergeCell ref="A176:A178"/>
-    <mergeCell ref="A173:A175"/>
-    <mergeCell ref="A170:A172"/>
-    <mergeCell ref="A166:A169"/>
-    <mergeCell ref="B203:B204"/>
-    <mergeCell ref="A203:A204"/>
-    <mergeCell ref="A112:A113"/>
-    <mergeCell ref="B103:B105"/>
-    <mergeCell ref="B98:B102"/>
-    <mergeCell ref="B96:B97"/>
-    <mergeCell ref="B89:B92"/>
-    <mergeCell ref="B85:B88"/>
-    <mergeCell ref="F85:F88"/>
-    <mergeCell ref="F89:F92"/>
-    <mergeCell ref="A16:A19"/>
-    <mergeCell ref="B70:B74"/>
-    <mergeCell ref="B75:B77"/>
-    <mergeCell ref="B78:B82"/>
-    <mergeCell ref="B83:B84"/>
-    <mergeCell ref="B55:B57"/>
-    <mergeCell ref="B68:B69"/>
-    <mergeCell ref="B64:B67"/>
-    <mergeCell ref="B58:B63"/>
-    <mergeCell ref="B49:B51"/>
-    <mergeCell ref="A49:A51"/>
-    <mergeCell ref="B52:B54"/>
-    <mergeCell ref="A52:A54"/>
-    <mergeCell ref="F70:F74"/>
-    <mergeCell ref="F75:F77"/>
-    <mergeCell ref="F78:F82"/>
-    <mergeCell ref="F83:F84"/>
-    <mergeCell ref="F176:F178"/>
-    <mergeCell ref="F193:F196"/>
-    <mergeCell ref="B193:B196"/>
-    <mergeCell ref="B176:B178"/>
-    <mergeCell ref="F155:F158"/>
-    <mergeCell ref="F159:F160"/>
-    <mergeCell ref="F161:F165"/>
-    <mergeCell ref="F166:F169"/>
-    <mergeCell ref="F170:F172"/>
-    <mergeCell ref="F173:F175"/>
-    <mergeCell ref="B173:B175"/>
-    <mergeCell ref="B170:B172"/>
-    <mergeCell ref="B166:B169"/>
-    <mergeCell ref="B161:B165"/>
-    <mergeCell ref="B159:B160"/>
+    <mergeCell ref="A45:A48"/>
+    <mergeCell ref="B132:B133"/>
+    <mergeCell ref="A132:A133"/>
+    <mergeCell ref="B134:B136"/>
+    <mergeCell ref="A134:A136"/>
+    <mergeCell ref="B137:B139"/>
+    <mergeCell ref="A137:A139"/>
+    <mergeCell ref="B124:B126"/>
+    <mergeCell ref="A124:A126"/>
+    <mergeCell ref="B127:B129"/>
+    <mergeCell ref="A127:A129"/>
+    <mergeCell ref="B130:B131"/>
+    <mergeCell ref="A130:A131"/>
+    <mergeCell ref="B114:B118"/>
+    <mergeCell ref="A114:A118"/>
+    <mergeCell ref="B119:B121"/>
+    <mergeCell ref="A119:A121"/>
+    <mergeCell ref="B122:B123"/>
+    <mergeCell ref="A122:A123"/>
+    <mergeCell ref="B207:B208"/>
+    <mergeCell ref="A207:A208"/>
+    <mergeCell ref="A199:A202"/>
+    <mergeCell ref="B199:B202"/>
+    <mergeCell ref="A180:A181"/>
+    <mergeCell ref="B180:B181"/>
+    <mergeCell ref="A183:A184"/>
+    <mergeCell ref="B183:B184"/>
+    <mergeCell ref="B185:B187"/>
+    <mergeCell ref="A185:A187"/>
+    <mergeCell ref="B189:B191"/>
+    <mergeCell ref="A189:A191"/>
+    <mergeCell ref="B155:B158"/>
+    <mergeCell ref="B141:B143"/>
+    <mergeCell ref="A141:A143"/>
+    <mergeCell ref="F2:F7"/>
+    <mergeCell ref="B2:B7"/>
+    <mergeCell ref="A2:A7"/>
+    <mergeCell ref="F8:F11"/>
+    <mergeCell ref="F12:F15"/>
+    <mergeCell ref="B12:B15"/>
+    <mergeCell ref="B8:B11"/>
+    <mergeCell ref="A8:A11"/>
+    <mergeCell ref="A12:A15"/>
     <mergeCell ref="F16:F19"/>
     <mergeCell ref="B16:B19"/>
     <mergeCell ref="F153:F154"/>
@@ -4862,38 +4855,32 @@
     <mergeCell ref="B112:B113"/>
     <mergeCell ref="B109:B111"/>
     <mergeCell ref="B106:B108"/>
-    <mergeCell ref="F2:F7"/>
-    <mergeCell ref="B2:B7"/>
-    <mergeCell ref="A2:A7"/>
-    <mergeCell ref="F8:F11"/>
-    <mergeCell ref="F12:F15"/>
-    <mergeCell ref="B12:B15"/>
-    <mergeCell ref="B8:B11"/>
-    <mergeCell ref="A8:A11"/>
-    <mergeCell ref="A12:A15"/>
-    <mergeCell ref="B130:B131"/>
-    <mergeCell ref="A130:A131"/>
-    <mergeCell ref="B114:B118"/>
-    <mergeCell ref="A114:A118"/>
-    <mergeCell ref="B119:B121"/>
-    <mergeCell ref="A119:A121"/>
-    <mergeCell ref="B122:B123"/>
-    <mergeCell ref="A122:A123"/>
-    <mergeCell ref="B207:B208"/>
-    <mergeCell ref="A207:A208"/>
-    <mergeCell ref="A199:A202"/>
-    <mergeCell ref="B199:B202"/>
-    <mergeCell ref="A180:A181"/>
-    <mergeCell ref="B180:B181"/>
-    <mergeCell ref="A183:A184"/>
-    <mergeCell ref="B183:B184"/>
-    <mergeCell ref="B185:B187"/>
-    <mergeCell ref="A185:A187"/>
-    <mergeCell ref="B189:B191"/>
-    <mergeCell ref="A189:A191"/>
-    <mergeCell ref="B155:B158"/>
-    <mergeCell ref="B141:B143"/>
-    <mergeCell ref="A141:A143"/>
+    <mergeCell ref="B193:B196"/>
+    <mergeCell ref="B176:B178"/>
+    <mergeCell ref="F155:F158"/>
+    <mergeCell ref="F159:F160"/>
+    <mergeCell ref="F161:F165"/>
+    <mergeCell ref="F166:F169"/>
+    <mergeCell ref="F170:F172"/>
+    <mergeCell ref="F173:F175"/>
+    <mergeCell ref="B173:B175"/>
+    <mergeCell ref="B170:B172"/>
+    <mergeCell ref="B166:B169"/>
+    <mergeCell ref="B161:B165"/>
+    <mergeCell ref="B159:B160"/>
+    <mergeCell ref="A16:A19"/>
+    <mergeCell ref="B70:B74"/>
+    <mergeCell ref="B75:B77"/>
+    <mergeCell ref="B78:B82"/>
+    <mergeCell ref="B83:B84"/>
+    <mergeCell ref="B55:B57"/>
+    <mergeCell ref="B68:B69"/>
+    <mergeCell ref="B64:B67"/>
+    <mergeCell ref="B58:B63"/>
+    <mergeCell ref="B49:B51"/>
+    <mergeCell ref="A49:A51"/>
+    <mergeCell ref="B52:B54"/>
+    <mergeCell ref="A52:A54"/>
     <mergeCell ref="B20:B26"/>
     <mergeCell ref="A20:A26"/>
     <mergeCell ref="B27:B29"/>
@@ -4905,17 +4892,30 @@
     <mergeCell ref="B40:B44"/>
     <mergeCell ref="A40:A44"/>
     <mergeCell ref="B45:B48"/>
-    <mergeCell ref="A45:A48"/>
-    <mergeCell ref="B132:B133"/>
-    <mergeCell ref="A132:A133"/>
-    <mergeCell ref="B134:B136"/>
-    <mergeCell ref="A134:A136"/>
-    <mergeCell ref="B137:B139"/>
-    <mergeCell ref="A137:A139"/>
-    <mergeCell ref="B124:B126"/>
-    <mergeCell ref="A124:A126"/>
-    <mergeCell ref="B127:B129"/>
-    <mergeCell ref="A127:A129"/>
+    <mergeCell ref="F55:F57"/>
+    <mergeCell ref="F58:F63"/>
+    <mergeCell ref="F68:F69"/>
+    <mergeCell ref="A193:A196"/>
+    <mergeCell ref="A176:A178"/>
+    <mergeCell ref="A173:A175"/>
+    <mergeCell ref="A170:A172"/>
+    <mergeCell ref="A166:A169"/>
+    <mergeCell ref="B203:B204"/>
+    <mergeCell ref="A203:A204"/>
+    <mergeCell ref="A112:A113"/>
+    <mergeCell ref="B103:B105"/>
+    <mergeCell ref="B98:B102"/>
+    <mergeCell ref="B96:B97"/>
+    <mergeCell ref="B89:B92"/>
+    <mergeCell ref="B85:B88"/>
+    <mergeCell ref="F85:F88"/>
+    <mergeCell ref="F89:F92"/>
+    <mergeCell ref="F70:F74"/>
+    <mergeCell ref="F75:F77"/>
+    <mergeCell ref="F78:F82"/>
+    <mergeCell ref="F83:F84"/>
+    <mergeCell ref="F176:F178"/>
+    <mergeCell ref="F193:F196"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="C1:C1048576">

</xml_diff>